<commit_message>
add data, graph for 1gbps resnet101 in rack, uneven, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/1gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/resnet-101/graphs/1gbps_inrack_uneven_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.4461</c:v>
+                    <c:v>0.1747</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5118</c:v>
+                    <c:v>0.3792</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0784</c:v>
+                    <c:v>0.1481</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2413</c:v>
+                    <c:v>0.226</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0683</c:v>
+                    <c:v>0.0933</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0038</c:v>
+                    <c:v>0.002</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2945</c:v>
+                    <c:v>0.0074</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1647</c:v>
+                    <c:v>0.0391</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.273</c:v>
+                    <c:v>0.6695</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.345</c:v>
+                    <c:v>0.1916</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>23.0714</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.9421</c:v>
+                  <c:v>35.9416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.897</c:v>
+                  <c:v>42.8266</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.2283</c:v>
+                  <c:v>46.2611</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.0995</c:v>
+                  <c:v>48.0107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.9308</c:v>
+                    <c:v>0.5473</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0017</c:v>
+                    <c:v>0.0047</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1239</c:v>
+                    <c:v>0.1223</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2791</c:v>
+                    <c:v>0.1647</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0735</c:v>
+                    <c:v>0.1249</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0063</c:v>
+                    <c:v>0.2472</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3165</c:v>
+                    <c:v>0.3123</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7025</c:v>
+                    <c:v>0.7028</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0929</c:v>
+                    <c:v>0.8227</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4449</c:v>
+                    <c:v>0.1308</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.71</c:v>
+                  <c:v>3.0966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.891</c:v>
+                  <c:v>25.8893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.8137</c:v>
+                  <c:v>37.8151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.594</c:v>
+                  <c:v>43.6009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.729</c:v>
+                  <c:v>46.8277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1709</c:v>
+                    <c:v>0.2534</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0005</c:v>
+                    <c:v>0.0025</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.5541</c:v>
+                    <c:v>0.4575</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5784</c:v>
+                    <c:v>0.5663</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1542</c:v>
+                    <c:v>0.5621</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1603</c:v>
+                    <c:v>0.1605</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4615</c:v>
+                    <c:v>0.4595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9779</c:v>
+                    <c:v>1.0896</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3235</c:v>
+                    <c:v>1.3668</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9835</c:v>
+                    <c:v>1.1017</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1394</c:v>
+                  <c:v>0.1047</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.6382</c:v>
+                  <c:v>21.6362</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.2124</c:v>
+                  <c:v>34.3055</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.3465</c:v>
+                  <c:v>41.4308</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.5031</c:v>
+                  <c:v>45.3169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0068</c:v>
+                    <c:v>0.1155</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1646</c:v>
+                    <c:v>0.0232</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6989</c:v>
+                    <c:v>0.4602</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1105</c:v>
+                    <c:v>0.3819</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1261</c:v>
+                    <c:v>0.2138</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0238</c:v>
+                    <c:v>0.0035</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3041</c:v>
+                    <c:v>0.4489</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0169</c:v>
+                    <c:v>1.2657</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9728</c:v>
+                    <c:v>3.3725</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.1913</c:v>
+                    <c:v>0.0595</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.2301</c:v>
+                  <c:v>21.3749</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33.9329</c:v>
+                  <c:v>34.1637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.5493</c:v>
+                  <c:v>41.6299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.4454</c:v>
+                  <c:v>45.4972</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2042542112"/>
-        <c:axId val="-2042535888"/>
+        <c:axId val="-2015921184"/>
+        <c:axId val="-2015823312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2042542112"/>
+        <c:axId val="-2015921184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042535888"/>
+        <c:crossAx val="-2015823312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2042535888"/>
+        <c:axId val="-2015823312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042542112"/>
+        <c:crossAx val="-2015921184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1296,16 +1293,16 @@
                     <c:v>0.0017</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0003</c:v>
+                    <c:v>0.0009</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4956</c:v>
+                    <c:v>0.2062</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3977</c:v>
+                    <c:v>0.2084</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1320,16 +1317,16 @@
                     <c:v>0.0031</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0004</c:v>
+                    <c:v>0.0012</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0006</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.263</c:v>
+                    <c:v>0.3874</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4683</c:v>
+                    <c:v>0.1867</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1388,10 +1385,10 @@
                   <c:v>43.738</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.8652</c:v>
+                  <c:v>47.0714</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.4566</c:v>
+                  <c:v>48.4882</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1948</c:v>
+                    <c:v>0.1954</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0017</c:v>
+                    <c:v>0.0043</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0024</c:v>
+                    <c:v>0.0014</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3617</c:v>
+                    <c:v>0.0713</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1717</c:v>
+                    <c:v>0.4033</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2868</c:v>
+                    <c:v>0.7436</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0012</c:v>
+                    <c:v>0.0013</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0034</c:v>
+                    <c:v>0.002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3632</c:v>
+                    <c:v>0.3762</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2776</c:v>
+                    <c:v>0.1777</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,19 +1523,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.8255</c:v>
+                  <c:v>2.0203</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.9045</c:v>
+                  <c:v>25.9058</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>37.9495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.9739</c:v>
+                  <c:v>43.9731</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.9864</c:v>
+                  <c:v>46.9867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2198</c:v>
+                    <c:v>0.2434</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.2039</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2667</c:v>
+                    <c:v>0.2489</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>2.4109</c:v>
+                    <c:v>0.7562</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5166</c:v>
+                    <c:v>1.2842</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.143</c:v>
+                    <c:v>0.3033</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0025</c:v>
+                    <c:v>0.4251</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1101</c:v>
+                    <c:v>0.2856</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6353</c:v>
+                    <c:v>0.1381</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8992</c:v>
+                    <c:v>0.9033</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1679,13 +1676,13 @@
                   <c:v>8.1001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.6253</c:v>
+                  <c:v>27.6231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.8687</c:v>
+                  <c:v>38.7351</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.8197</c:v>
+                  <c:v>44.1445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,16 +1734,16 @@
                     <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.017</c:v>
+                    <c:v>0.1867</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0867</c:v>
+                    <c:v>0.1476</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6488</c:v>
+                    <c:v>0.5715</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9017</c:v>
+                    <c:v>0.6482</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0239</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1918</c:v>
+                    <c:v>0.2277</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1888</c:v>
+                    <c:v>0.1598</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5132</c:v>
+                    <c:v>1.8826</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7248</c:v>
+                    <c:v>0.745</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1823,16 +1820,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.823</c:v>
+                  <c:v>5.8541</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.3842</c:v>
+                  <c:v>26.2477</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.7334</c:v>
+                  <c:v>37.8152</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.4333</c:v>
+                  <c:v>44.3799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2042456688"/>
-        <c:axId val="-2042450464"/>
+        <c:axId val="-2044885088"/>
+        <c:axId val="-2044850048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2042456688"/>
+        <c:axId val="-2044885088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042450464"/>
+        <c:crossAx val="-2044850048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2042450464"/>
+        <c:axId val="-2044850048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042456688"/>
+        <c:crossAx val="-2044885088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0187</c:v>
+                    <c:v>0.291</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0134</c:v>
+                    <c:v>0.3781</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0761</c:v>
+                    <c:v>0.2381</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0825</c:v>
+                    <c:v>0.0156</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0258</c:v>
+                    <c:v>0.018</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1538</c:v>
+                    <c:v>0.0032</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0009</c:v>
+                    <c:v>0.0012</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1102</c:v>
+                    <c:v>0.1533</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1588</c:v>
+                    <c:v>0.3739</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1634</c:v>
+                    <c:v>0.0315</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>48.1998</c:v>
+                  <c:v>48.0492</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.4235</c:v>
+                  <c:v>73.424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.6358</c:v>
+                  <c:v>86.617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.2987</c:v>
+                  <c:v>93.2848</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.6302</c:v>
+                  <c:v>96.60850000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.525</c:v>
+                    <c:v>0.5395</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0017</c:v>
+                    <c:v>0.0025</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1255</c:v>
+                    <c:v>0.1249</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1039</c:v>
+                    <c:v>0.1578</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.046</c:v>
+                    <c:v>0.2518</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0114</c:v>
+                    <c:v>0.2451</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3161</c:v>
+                    <c:v>0.3144</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6999</c:v>
+                    <c:v>0.6997</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2458</c:v>
+                    <c:v>0.1861</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1897</c:v>
+                    <c:v>0.3709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.9378</c:v>
+                  <c:v>4.9264</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>51.7955</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.7615</c:v>
+                  <c:v>75.7617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.7744</c:v>
+                  <c:v>87.7546</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.8798</c:v>
+                  <c:v>93.69970000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1709</c:v>
+                    <c:v>0.2431</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0032</c:v>
+                    <c:v>0.005</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4831</c:v>
+                    <c:v>0.3862</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.507</c:v>
+                    <c:v>0.2544</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1241</c:v>
+                    <c:v>0.1964</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1603</c:v>
+                    <c:v>0.1359</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4613</c:v>
+                    <c:v>0.4595</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9494</c:v>
+                    <c:v>1.0541</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9537</c:v>
+                    <c:v>0.8657</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0782</c:v>
+                    <c:v>0.7579</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2705,19 +2702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1394</c:v>
+                  <c:v>0.115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.7356</c:v>
+                  <c:v>29.7338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.7992</c:v>
+                  <c:v>61.893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.8386</c:v>
+                  <c:v>80.1175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.7784</c:v>
+                  <c:v>89.7373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0034</c:v>
+                    <c:v>0.1155</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1551</c:v>
+                    <c:v>0.0228</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4989</c:v>
+                    <c:v>0.3925</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0358</c:v>
+                    <c:v>0.3202</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.275</c:v>
+                    <c:v>0.1256</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0238</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3136</c:v>
+                    <c:v>0.4464</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0555</c:v>
+                    <c:v>1.1681</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2579</c:v>
+                    <c:v>2.3847</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.589</c:v>
+                    <c:v>0.3447</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0034</c:v>
+                  <c:v>-0.0204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.0651</c:v>
+                  <c:v>27.1979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.4051</c:v>
+                  <c:v>60.5068</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.4829</c:v>
+                  <c:v>79.3172</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89.315</c:v>
+                  <c:v>89.4175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2042371824"/>
-        <c:axId val="-2042365600"/>
+        <c:axId val="-2045170640"/>
+        <c:axId val="-2044810496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2042371824"/>
+        <c:axId val="-2045170640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042365600"/>
+        <c:crossAx val="-2044810496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2042365600"/>
+        <c:axId val="-2044810496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042371824"/>
+        <c:crossAx val="-2045170640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3357,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0253</c:v>
+                    <c:v>0.3894</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0216</c:v>
+                    <c:v>0.604</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1351</c:v>
+                    <c:v>0.4231</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.099</c:v>
+                    <c:v>0.133</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0105</c:v>
+                    <c:v>0.0664</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3381,19 +3378,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2035</c:v>
+                    <c:v>0.0043</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0014</c:v>
+                    <c:v>0.0026</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1957</c:v>
+                    <c:v>0.2725</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2983</c:v>
+                    <c:v>0.7471</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3156</c:v>
+                    <c:v>0.0477</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3443,19 +3440,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>30.9533</c:v>
+                  <c:v>30.7525</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.4895</c:v>
+                  <c:v>57.4913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.2466</c:v>
+                  <c:v>76.2131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.3876</c:v>
+                  <c:v>87.301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.4607</c:v>
+                  <c:v>93.405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,19 +3501,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5446</c:v>
+                    <c:v>0.2859</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0022</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1986</c:v>
+                    <c:v>0.2002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1249</c:v>
+                    <c:v>0.1851</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1234</c:v>
+                    <c:v>0.3875</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3528,19 +3525,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2042</c:v>
+                    <c:v>0.2635</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.4255</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1296</c:v>
+                    <c:v>1.1297</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4991</c:v>
+                    <c:v>0.3572</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3965</c:v>
+                    <c:v>0.7589</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3590,19 +3587,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.1702</c:v>
+                  <c:v>3.1627</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>34.9428</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60.9396</c:v>
+                  <c:v>60.9391</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.2392</c:v>
+                  <c:v>78.2403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.4554</c:v>
+                  <c:v>88.1156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3651,19 +3648,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.185</c:v>
+                    <c:v>0.2913</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0033</c:v>
+                    <c:v>0.0137</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7599</c:v>
+                    <c:v>0.3284</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2645</c:v>
+                    <c:v>0.5603</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.0573</c:v>
+                    <c:v>0.1899</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3675,19 +3672,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0764</c:v>
+                    <c:v>0.0003</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.6733</c:v>
+                    <c:v>0.6629</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.4937</c:v>
+                    <c:v>1.8501</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.515</c:v>
+                    <c:v>1.2708</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3921</c:v>
+                    <c:v>1.4548</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3737,19 +3734,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1219</c:v>
+                  <c:v>0.1153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.5426</c:v>
+                  <c:v>23.5322</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.1998</c:v>
+                  <c:v>47.5562</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.9955</c:v>
+                  <c:v>67.4045</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.9341</c:v>
+                  <c:v>81.5956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3798,19 +3795,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0034</c:v>
+                    <c:v>0.0917</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0073</c:v>
+                    <c:v>0.1786</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.7411</c:v>
+                    <c:v>0.4026</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3426</c:v>
+                    <c:v>0.537</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3506</c:v>
+                    <c:v>0.5042</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3825,16 +3822,16 @@
                     <c:v>0.0238</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4904</c:v>
+                    <c:v>0.3191</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2389</c:v>
+                    <c:v>1.6564</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0696</c:v>
+                    <c:v>2.7447</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0084</c:v>
+                    <c:v>0.3199</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3887,16 +3884,16 @@
                   <c:v>0.0034</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.7129</c:v>
+                  <c:v>22.5416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46.1508</c:v>
+                  <c:v>46.5673</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.7607</c:v>
+                  <c:v>66.7397</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.15179999999999</c:v>
+                  <c:v>80.9334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2042225968"/>
-        <c:axId val="-2042200496"/>
+        <c:axId val="-2022539968"/>
+        <c:axId val="-2029564800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2042225968"/>
+        <c:axId val="-2022539968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042200496"/>
+        <c:crossAx val="-2029564800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2042200496"/>
+        <c:axId val="-2029564800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042225968"/>
+        <c:crossAx val="-2022539968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>0</v>
-          </cell>
-          <cell r="G4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>17.238099999999999</v>
-          </cell>
-          <cell r="F5">
-            <v>0.85809999999999997</v>
-          </cell>
-          <cell r="G5">
-            <v>0.26169999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>39.0169</v>
-          </cell>
-          <cell r="F6">
-            <v>5.5888</v>
-          </cell>
-          <cell r="G6">
-            <v>3.6522999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>37.7652</v>
-          </cell>
-          <cell r="F7">
-            <v>0.91710000000000003</v>
-          </cell>
-          <cell r="G7">
-            <v>3.9735</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>43.6539</v>
-          </cell>
-          <cell r="F8">
-            <v>0.1651</v>
-          </cell>
-          <cell r="G8">
-            <v>1.8986000000000001</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>0</v>
-          </cell>
-          <cell r="F10">
-            <v>0.26300000000000001</v>
-          </cell>
-          <cell r="G10">
-            <v>0.19209999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>0</v>
-          </cell>
-          <cell r="G11">
-            <v>0.13550000000000001</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>28.887499999999999</v>
-          </cell>
-          <cell r="F12">
-            <v>11.911099999999999</v>
-          </cell>
-          <cell r="G12">
-            <v>7.1414999999999997</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>24.7256</v>
-          </cell>
-          <cell r="F13">
-            <v>1.6279999999999999</v>
-          </cell>
-          <cell r="G13">
-            <v>12.668100000000001</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>37.367199999999997</v>
-          </cell>
-          <cell r="F14">
-            <v>0.79590000000000005</v>
-          </cell>
-          <cell r="G14">
-            <v>2.649</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>0</v>
-          </cell>
-          <cell r="G16">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>0.24340000000000001</v>
-          </cell>
-          <cell r="G17">
-            <v>0.26779999999999998</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>8.0200999999999993</v>
-          </cell>
-          <cell r="F18">
-            <v>8.0200999999999993</v>
-          </cell>
-          <cell r="G18">
-            <v>14.3773</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>3.4820000000000002</v>
-          </cell>
-          <cell r="F19">
-            <v>7.3723000000000001</v>
-          </cell>
-          <cell r="G19">
-            <v>12.925599999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>24.358799999999999</v>
-          </cell>
-          <cell r="F20">
-            <v>5.7351999999999999</v>
-          </cell>
-          <cell r="G20">
-            <v>2.1141000000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>0</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>0.1153</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>-2.86E-2</v>
-          </cell>
-          <cell r="F24">
-            <v>0.2611</v>
-          </cell>
-          <cell r="G24">
-            <v>0.21970000000000001</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-22.630199999999999</v>
-          </cell>
-          <cell r="F25">
-            <v>7.0137999999999998</v>
-          </cell>
-          <cell r="G25">
-            <v>46.412399999999998</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>2.1263999999999998</v>
-          </cell>
-          <cell r="F26">
-            <v>2.6492</v>
-          </cell>
-          <cell r="G26">
-            <v>10.610300000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F29">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G29">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>21.983799999999999</v>
-          </cell>
-          <cell r="F30">
-            <v>0</v>
-          </cell>
-          <cell r="G30">
-            <v>1.04E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>35.973199999999999</v>
-          </cell>
-          <cell r="F31">
-            <v>1.41E-2</v>
-          </cell>
-          <cell r="G31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>43.075600000000001</v>
-          </cell>
-          <cell r="F32">
-            <v>8.9700000000000002E-2</v>
-          </cell>
-          <cell r="G32">
-            <v>0.45300000000000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>46.816899999999997</v>
-          </cell>
-          <cell r="F33">
-            <v>0.60450000000000004</v>
-          </cell>
-          <cell r="G33">
-            <v>0.50980000000000003</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>0.3841</v>
-          </cell>
-          <cell r="F35">
-            <v>0.19589999999999999</v>
-          </cell>
-          <cell r="G35">
-            <v>7.7299999999999994E-2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>-5.0045000000000002</v>
-          </cell>
-          <cell r="F36">
-            <v>3.7900000000000003E-2</v>
-          </cell>
-          <cell r="G36">
-            <v>0.12720000000000001</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>21.983799999999999</v>
-          </cell>
-          <cell r="F37">
-            <v>0.1396</v>
-          </cell>
-          <cell r="G37">
-            <v>0.1087</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>35.933900000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>0.15570000000000001</v>
-          </cell>
-          <cell r="G38">
-            <v>0.6431</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>43.1629</v>
-          </cell>
-          <cell r="F39">
-            <v>0.13739999999999999</v>
-          </cell>
-          <cell r="G39">
-            <v>0.37040000000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F42">
-            <v>2.86E-2</v>
-          </cell>
-          <cell r="G42">
-            <v>0.2636</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>-5.7415000000000003</v>
-          </cell>
-          <cell r="F43">
-            <v>0.19089999999999999</v>
-          </cell>
-          <cell r="G43">
-            <v>0.74450000000000005</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>21.6325</v>
-          </cell>
-          <cell r="F44">
-            <v>12.7317</v>
-          </cell>
-          <cell r="G44">
-            <v>2.7587999999999999</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>36.095399999999998</v>
-          </cell>
-          <cell r="F45">
-            <v>0.41839999999999999</v>
-          </cell>
-          <cell r="G45">
-            <v>0.28089999999999998</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>0</v>
-          </cell>
-          <cell r="F48">
-            <v>0</v>
-          </cell>
-          <cell r="G48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>0.33560000000000001</v>
-          </cell>
-          <cell r="F49">
-            <v>9.2899999999999996E-2</v>
-          </cell>
-          <cell r="G49">
-            <v>0.40639999999999998</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>-8.2013999999999996</v>
-          </cell>
-          <cell r="F50">
-            <v>42.866500000000002</v>
-          </cell>
-          <cell r="G50">
-            <v>5.8691000000000004</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>21.259899999999998</v>
-          </cell>
-          <cell r="F51">
-            <v>9.0968999999999998</v>
-          </cell>
-          <cell r="G51">
-            <v>2.1303999999999998</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>-3.8346</v>
-          </cell>
-          <cell r="F54">
-            <v>0.52749999999999997</v>
-          </cell>
-          <cell r="G54">
-            <v>0.10730000000000001</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>39.221800000000002</v>
-          </cell>
-          <cell r="F55">
-            <v>0.83879999999999999</v>
-          </cell>
-          <cell r="G55">
-            <v>0.26179999999999998</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>74.990200000000002</v>
-          </cell>
-          <cell r="F56">
-            <v>5.5888999999999998</v>
-          </cell>
-          <cell r="G56">
-            <v>3.3757999999999999</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>80.340999999999994</v>
-          </cell>
-          <cell r="F57">
-            <v>2.9379</v>
-          </cell>
-          <cell r="G57">
-            <v>4.26</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>90.113900000000001</v>
-          </cell>
-          <cell r="F58">
-            <v>1.6204000000000001</v>
-          </cell>
-          <cell r="G58">
-            <v>0.89080000000000004</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>0.3841</v>
-          </cell>
-          <cell r="F60">
-            <v>0.19589999999999999</v>
-          </cell>
-          <cell r="G60">
-            <v>7.7299999999999994E-2</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>-5.0045000000000002</v>
-          </cell>
-          <cell r="F61">
-            <v>3.7900000000000003E-2</v>
-          </cell>
-          <cell r="G61">
-            <v>0.12720000000000001</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>50.832000000000001</v>
-          </cell>
-          <cell r="F62">
-            <v>11.8719</v>
-          </cell>
-          <cell r="G62">
-            <v>7.1719999999999997</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>64.251800000000003</v>
-          </cell>
-          <cell r="F63">
-            <v>3.6684999999999999</v>
-          </cell>
-          <cell r="G63">
-            <v>5.6044</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>80.218699999999998</v>
-          </cell>
-          <cell r="F64">
-            <v>3.2532000000000001</v>
-          </cell>
-          <cell r="G64">
-            <v>2.5999999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0</v>
-          </cell>
-          <cell r="F66">
-            <v>0</v>
-          </cell>
-          <cell r="G66">
-            <v>0.1724</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>0.27200000000000002</v>
-          </cell>
-          <cell r="F67">
-            <v>2.86E-2</v>
-          </cell>
-          <cell r="G67">
-            <v>0.2636</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>2.2519</v>
-          </cell>
-          <cell r="F68">
-            <v>7.2564000000000002</v>
-          </cell>
-          <cell r="G68">
-            <v>14.3772</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>24.073699999999999</v>
-          </cell>
-          <cell r="F69">
-            <v>4.8856000000000002</v>
-          </cell>
-          <cell r="G69">
-            <v>14.556699999999999</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>61.642499999999998</v>
-          </cell>
-          <cell r="F70">
-            <v>2.1135999999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>3.7351999999999999</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>0</v>
-          </cell>
-          <cell r="F73">
-            <v>0</v>
-          </cell>
-          <cell r="G73">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>0.33560000000000001</v>
-          </cell>
-          <cell r="F74">
-            <v>9.2899999999999996E-2</v>
-          </cell>
-          <cell r="G74">
-            <v>0.40639999999999998</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>-15.534700000000001</v>
-          </cell>
-          <cell r="F75">
-            <v>21.0212</v>
-          </cell>
-          <cell r="G75">
-            <v>45.945999999999998</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>21.519100000000002</v>
-          </cell>
-          <cell r="F76">
-            <v>11.7506</v>
-          </cell>
-          <cell r="G76">
-            <v>3.4872999999999998</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>22.095500000000001</v>
-          </cell>
-          <cell r="F80">
-            <v>1.0859000000000001</v>
-          </cell>
-          <cell r="G80">
-            <v>0.33550000000000002</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>60.938499999999998</v>
-          </cell>
-          <cell r="F81">
-            <v>8.7289999999999992</v>
-          </cell>
-          <cell r="G81">
-            <v>5.2798999999999996</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>65.484899999999996</v>
-          </cell>
-          <cell r="F82">
-            <v>5.2960000000000003</v>
-          </cell>
-          <cell r="G82">
-            <v>7.3456999999999999</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>81.555199999999999</v>
-          </cell>
-          <cell r="F83">
-            <v>3.2852000000000001</v>
-          </cell>
-          <cell r="G83">
-            <v>1.3673</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>36.889200000000002</v>
-          </cell>
-          <cell r="F87">
-            <v>15.129200000000001</v>
-          </cell>
-          <cell r="G87">
-            <v>9.2810000000000006</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>44.071300000000001</v>
-          </cell>
-          <cell r="F88">
-            <v>6.0250000000000004</v>
-          </cell>
-          <cell r="G88">
-            <v>8.9834999999999994</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>64.968299999999999</v>
-          </cell>
-          <cell r="F89">
-            <v>5.4389000000000003</v>
-          </cell>
-          <cell r="G89">
-            <v>0.2442</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>7.5978000000000003</v>
-          </cell>
-          <cell r="F93">
-            <v>7.5978000000000003</v>
-          </cell>
-          <cell r="G93">
-            <v>13.578099999999999</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>4.1816000000000004</v>
-          </cell>
-          <cell r="F94">
-            <v>7.3007</v>
-          </cell>
-          <cell r="G94">
-            <v>19.327999999999999</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>39.947899999999997</v>
-          </cell>
-          <cell r="F95">
-            <v>2.8664000000000001</v>
-          </cell>
-          <cell r="G95">
-            <v>5.8739999999999997</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>13.1912</v>
-          </cell>
-          <cell r="F100">
-            <v>43.831099999999999</v>
-          </cell>
-          <cell r="G100">
-            <v>18.806100000000001</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>-1.0195000000000001</v>
-          </cell>
-          <cell r="F101">
-            <v>10.539300000000001</v>
-          </cell>
-          <cell r="G101">
-            <v>15.641400000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6874,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:G101"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,10 +6941,10 @@
         <v>23.071400000000001</v>
       </c>
       <c r="F4">
-        <v>3.8E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G4">
-        <v>0.4461</v>
+        <v>0.17469999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>35.942100000000003</v>
+        <v>35.941600000000001</v>
       </c>
       <c r="F5">
-        <v>0.29449999999999998</v>
+        <v>7.4000000000000003E-3</v>
       </c>
       <c r="G5">
-        <v>0.51180000000000003</v>
+        <v>0.37919999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6984,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>42.896999999999998</v>
+        <v>42.826599999999999</v>
       </c>
       <c r="F6">
-        <v>0.16470000000000001</v>
+        <v>3.9100000000000003E-2</v>
       </c>
       <c r="G6">
-        <v>7.8399999999999997E-2</v>
+        <v>0.14810000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>46.228299999999997</v>
+        <v>46.261099999999999</v>
       </c>
       <c r="F7">
-        <v>0.27300000000000002</v>
+        <v>0.66949999999999998</v>
       </c>
       <c r="G7">
-        <v>0.24129999999999999</v>
+        <v>0.22600000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>48.099499999999999</v>
+        <v>48.0107</v>
       </c>
       <c r="F8">
-        <v>0.34499999999999997</v>
+        <v>0.19159999999999999</v>
       </c>
       <c r="G8">
-        <v>6.83E-2</v>
+        <v>9.3299999999999994E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>2.71</v>
+        <v>3.0966</v>
       </c>
       <c r="F10">
-        <v>6.3E-3</v>
+        <v>0.2472</v>
       </c>
       <c r="G10">
-        <v>0.93079999999999996</v>
+        <v>0.54730000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7988,13 +7076,13 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>25.890999999999998</v>
+        <v>25.889299999999999</v>
       </c>
       <c r="F11">
-        <v>0.3165</v>
+        <v>0.31230000000000002</v>
       </c>
       <c r="G11">
-        <v>1.6999999999999999E-3</v>
+        <v>4.7000000000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>37.813699999999997</v>
+        <v>37.815100000000001</v>
       </c>
       <c r="F12">
-        <v>0.70250000000000001</v>
+        <v>0.70279999999999998</v>
       </c>
       <c r="G12">
-        <v>0.1239</v>
+        <v>0.12230000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>43.594000000000001</v>
+        <v>43.600900000000003</v>
       </c>
       <c r="F13">
-        <v>9.2899999999999996E-2</v>
+        <v>0.82269999999999999</v>
       </c>
       <c r="G13">
-        <v>0.27910000000000001</v>
+        <v>0.16470000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>46.728999999999999</v>
+        <v>46.8277</v>
       </c>
       <c r="F14">
-        <v>0.44490000000000002</v>
+        <v>0.1308</v>
       </c>
       <c r="G14">
-        <v>7.3499999999999996E-2</v>
+        <v>0.1249</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,13 +7168,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0.1394</v>
+        <v>0.1047</v>
       </c>
       <c r="F16">
-        <v>0.1603</v>
+        <v>0.1605</v>
       </c>
       <c r="G16">
-        <v>0.1709</v>
+        <v>0.25340000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8103,13 +7191,13 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>21.638200000000001</v>
+        <v>21.636199999999999</v>
       </c>
       <c r="F17">
-        <v>0.46150000000000002</v>
+        <v>0.45950000000000002</v>
       </c>
       <c r="G17">
-        <v>5.0000000000000001E-4</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8126,13 +7214,13 @@
         <v>8</v>
       </c>
       <c r="E18">
-        <v>34.212400000000002</v>
+        <v>34.305500000000002</v>
       </c>
       <c r="F18">
-        <v>0.97789999999999999</v>
+        <v>1.0895999999999999</v>
       </c>
       <c r="G18">
-        <v>0.55410000000000004</v>
+        <v>0.45750000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>41.346499999999999</v>
+        <v>41.430799999999998</v>
       </c>
       <c r="F19">
-        <v>0.32350000000000001</v>
+        <v>1.3668</v>
       </c>
       <c r="G19">
-        <v>0.57840000000000003</v>
+        <v>0.56630000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>45.503100000000003</v>
+        <v>45.316899999999997</v>
       </c>
       <c r="F20">
-        <v>0.98350000000000004</v>
+        <v>1.1016999999999999</v>
       </c>
       <c r="G20">
-        <v>0.1542</v>
+        <v>0.56210000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8195,13 +7283,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>-2.0400000000000001E-2</v>
       </c>
       <c r="F22">
-        <v>2.3800000000000002E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="G22">
-        <v>6.7999999999999996E-3</v>
+        <v>0.11550000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7306,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>21.2301</v>
+        <v>21.3749</v>
       </c>
       <c r="F23">
-        <v>0.30409999999999998</v>
+        <v>0.44890000000000002</v>
       </c>
       <c r="G23">
-        <v>0.1646</v>
+        <v>2.3199999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8241,13 +7329,13 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <v>33.932899999999997</v>
+        <v>34.163699999999999</v>
       </c>
       <c r="F24">
-        <v>1.0168999999999999</v>
+        <v>1.2657</v>
       </c>
       <c r="G24">
-        <v>0.69889999999999997</v>
+        <v>0.4602</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>41.549300000000002</v>
+        <v>41.629899999999999</v>
       </c>
       <c r="F25">
-        <v>1.9728000000000001</v>
+        <v>3.3725000000000001</v>
       </c>
       <c r="G25">
-        <v>0.1105</v>
+        <v>0.38190000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>45.445399999999999</v>
+        <v>45.497199999999999</v>
       </c>
       <c r="F26">
-        <v>1.1913</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="G26">
-        <v>0.12609999999999999</v>
+        <v>0.21379999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8344,10 +7432,10 @@
         <v>37.482199999999999</v>
       </c>
       <c r="F30">
-        <v>4.0000000000000002E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G30">
-        <v>2.9999999999999997E-4</v>
+        <v>8.9999999999999998E-4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>46.865200000000002</v>
+        <v>47.071399999999997</v>
       </c>
       <c r="F32">
-        <v>0.26300000000000001</v>
+        <v>0.38740000000000002</v>
       </c>
       <c r="G32">
-        <v>0.49559999999999998</v>
+        <v>0.20619999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>48.456600000000002</v>
+        <v>48.488199999999999</v>
       </c>
       <c r="F33">
-        <v>0.46829999999999999</v>
+        <v>0.1867</v>
       </c>
       <c r="G33">
-        <v>0.3977</v>
+        <v>0.2084</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>1.8254999999999999</v>
+        <v>2.0203000000000002</v>
       </c>
       <c r="F35">
-        <v>0.2868</v>
+        <v>0.74360000000000004</v>
       </c>
       <c r="G35">
-        <v>0.1948</v>
+        <v>0.19539999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8456,13 +7544,13 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>25.904499999999999</v>
+        <v>25.905799999999999</v>
       </c>
       <c r="F36">
-        <v>1.1999999999999999E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G36">
-        <v>1.6999999999999999E-3</v>
+        <v>4.3E-3</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8482,10 +7570,10 @@
         <v>37.9495</v>
       </c>
       <c r="F37">
-        <v>3.3999999999999998E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="G37">
-        <v>2.3999999999999998E-3</v>
+        <v>1.4E-3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>43.9739</v>
+        <v>43.973100000000002</v>
       </c>
       <c r="F38">
-        <v>0.36320000000000002</v>
+        <v>0.37619999999999998</v>
       </c>
       <c r="G38">
-        <v>0.36170000000000002</v>
+        <v>7.1300000000000002E-2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>46.986400000000003</v>
+        <v>46.986699999999999</v>
       </c>
       <c r="F39">
-        <v>0.27760000000000001</v>
+        <v>0.1777</v>
       </c>
       <c r="G39">
-        <v>0.17169999999999999</v>
+        <v>0.40329999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8551,10 +7639,10 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0.14299999999999999</v>
+        <v>0.30330000000000001</v>
       </c>
       <c r="G41">
-        <v>0.2198</v>
+        <v>0.24340000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8574,7 +7662,7 @@
         <v>8.1000999999999994</v>
       </c>
       <c r="F42">
-        <v>2.5000000000000001E-3</v>
+        <v>0.42509999999999998</v>
       </c>
       <c r="G42">
         <v>0.2039</v>
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>27.625299999999999</v>
+        <v>27.623100000000001</v>
       </c>
       <c r="F43">
-        <v>0.1101</v>
+        <v>0.28560000000000002</v>
       </c>
       <c r="G43">
-        <v>0.26669999999999999</v>
+        <v>0.24890000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>39.868699999999997</v>
+        <v>38.735100000000003</v>
       </c>
       <c r="F44">
-        <v>1.6353</v>
+        <v>0.1381</v>
       </c>
       <c r="G44">
-        <v>2.4108999999999998</v>
+        <v>0.75619999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>43.819699999999997</v>
+        <v>44.144500000000001</v>
       </c>
       <c r="F45">
-        <v>0.8992</v>
+        <v>0.90329999999999999</v>
       </c>
       <c r="G45">
-        <v>0.51659999999999995</v>
+        <v>1.2842</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8666,7 +7754,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>2.3900000000000001E-2</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -8686,13 +7774,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>5.8230000000000004</v>
+        <v>5.8540999999999999</v>
       </c>
       <c r="F48">
-        <v>0.1918</v>
+        <v>0.22770000000000001</v>
       </c>
       <c r="G48">
-        <v>1.7000000000000001E-2</v>
+        <v>0.1867</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>26.3842</v>
+        <v>26.247699999999998</v>
       </c>
       <c r="F49">
-        <v>0.1888</v>
+        <v>0.1598</v>
       </c>
       <c r="G49">
-        <v>8.6699999999999999E-2</v>
+        <v>0.14760000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>37.733400000000003</v>
+        <v>37.815199999999997</v>
       </c>
       <c r="F50">
-        <v>0.51319999999999999</v>
+        <v>1.8826000000000001</v>
       </c>
       <c r="G50">
-        <v>0.64880000000000004</v>
+        <v>0.57150000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>43.433300000000003</v>
+        <v>44.379899999999999</v>
       </c>
       <c r="F51">
-        <v>0.7248</v>
+        <v>0.745</v>
       </c>
       <c r="G51">
-        <v>0.90169999999999995</v>
+        <v>0.6482</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>48.199800000000003</v>
+        <v>48.049199999999999</v>
       </c>
       <c r="F54">
-        <v>0.15379999999999999</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="G54">
-        <v>1.8700000000000001E-2</v>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>73.423500000000004</v>
+        <v>73.424000000000007</v>
       </c>
       <c r="F55">
-        <v>8.9999999999999998E-4</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="G55">
-        <v>1.34E-2</v>
+        <v>0.37809999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>86.635800000000003</v>
+        <v>86.617000000000004</v>
       </c>
       <c r="F56">
-        <v>0.11020000000000001</v>
+        <v>0.15329999999999999</v>
       </c>
       <c r="G56">
-        <v>7.6100000000000001E-2</v>
+        <v>0.23810000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>93.298699999999997</v>
+        <v>93.284800000000004</v>
       </c>
       <c r="F57">
-        <v>0.1588</v>
+        <v>0.37390000000000001</v>
       </c>
       <c r="G57">
-        <v>8.2500000000000004E-2</v>
+        <v>1.5599999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>96.630200000000002</v>
+        <v>96.608500000000006</v>
       </c>
       <c r="F58">
-        <v>0.16339999999999999</v>
+        <v>3.15E-2</v>
       </c>
       <c r="G58">
-        <v>2.58E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>4.9378000000000002</v>
+        <v>4.9264000000000001</v>
       </c>
       <c r="F60">
-        <v>1.14E-2</v>
+        <v>0.24510000000000001</v>
       </c>
       <c r="G60">
-        <v>0.52500000000000002</v>
+        <v>0.53949999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8927,10 +8015,10 @@
         <v>51.795499999999997</v>
       </c>
       <c r="F61">
-        <v>0.31609999999999999</v>
+        <v>0.31440000000000001</v>
       </c>
       <c r="G61">
-        <v>1.6999999999999999E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>75.761499999999998</v>
+        <v>75.761700000000005</v>
       </c>
       <c r="F62">
-        <v>0.69989999999999997</v>
+        <v>0.69969999999999999</v>
       </c>
       <c r="G62">
-        <v>0.1255</v>
+        <v>0.1249</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>87.7744</v>
+        <v>87.754599999999996</v>
       </c>
       <c r="F63">
-        <v>0.24579999999999999</v>
+        <v>0.18609999999999999</v>
       </c>
       <c r="G63">
-        <v>0.10390000000000001</v>
+        <v>0.1578</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>93.879800000000003</v>
+        <v>93.699700000000007</v>
       </c>
       <c r="F64">
-        <v>0.18970000000000001</v>
+        <v>0.37090000000000001</v>
       </c>
       <c r="G64">
-        <v>4.5999999999999999E-2</v>
+        <v>0.25180000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9016,13 +8104,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>0.1394</v>
+        <v>0.115</v>
       </c>
       <c r="F66">
-        <v>0.1603</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="G66">
-        <v>0.1709</v>
+        <v>0.24310000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>29.735600000000002</v>
+        <v>29.733799999999999</v>
       </c>
       <c r="F67">
-        <v>0.46129999999999999</v>
+        <v>0.45950000000000002</v>
       </c>
       <c r="G67">
-        <v>3.2000000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>61.799199999999999</v>
+        <v>61.893000000000001</v>
       </c>
       <c r="F68">
-        <v>0.94940000000000002</v>
+        <v>1.0541</v>
       </c>
       <c r="G68">
-        <v>0.48309999999999997</v>
+        <v>0.38619999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>79.8386</v>
+        <v>80.117500000000007</v>
       </c>
       <c r="F69">
-        <v>0.95369999999999999</v>
+        <v>0.86570000000000003</v>
       </c>
       <c r="G69">
-        <v>0.50700000000000001</v>
+        <v>0.25440000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>89.778400000000005</v>
+        <v>89.737300000000005</v>
       </c>
       <c r="F70">
-        <v>7.8200000000000006E-2</v>
+        <v>0.75790000000000002</v>
       </c>
       <c r="G70">
-        <v>0.1241</v>
+        <v>0.19639999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8219,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>3.3999999999999998E-3</v>
+        <v>-2.0400000000000001E-2</v>
       </c>
       <c r="F72">
-        <v>2.3800000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>3.3999999999999998E-3</v>
+        <v>0.11550000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8242,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>27.065100000000001</v>
+        <v>27.197900000000001</v>
       </c>
       <c r="F73">
-        <v>0.31359999999999999</v>
+        <v>0.44640000000000002</v>
       </c>
       <c r="G73">
-        <v>0.15509999999999999</v>
+        <v>2.2800000000000001E-2</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>60.405099999999997</v>
+        <v>60.506799999999998</v>
       </c>
       <c r="F74">
-        <v>1.0555000000000001</v>
+        <v>1.1680999999999999</v>
       </c>
       <c r="G74">
-        <v>0.49890000000000001</v>
+        <v>0.39250000000000002</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>79.482900000000001</v>
+        <v>79.3172</v>
       </c>
       <c r="F75">
-        <v>0.25790000000000002</v>
+        <v>2.3847</v>
       </c>
       <c r="G75">
-        <v>3.5799999999999998E-2</v>
+        <v>0.32019999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>89.314999999999998</v>
+        <v>89.417500000000004</v>
       </c>
       <c r="F76">
-        <v>0.58899999999999997</v>
+        <v>0.34470000000000001</v>
       </c>
       <c r="G76">
-        <v>0.27500000000000002</v>
+        <v>0.12559999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9251,13 +8339,13 @@
         <v>2</v>
       </c>
       <c r="E79">
-        <v>30.953299999999999</v>
+        <v>30.752500000000001</v>
       </c>
       <c r="F79">
-        <v>0.20349999999999999</v>
+        <v>4.3E-3</v>
       </c>
       <c r="G79">
-        <v>2.53E-2</v>
+        <v>0.38940000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,13 +8362,13 @@
         <v>4</v>
       </c>
       <c r="E80">
-        <v>57.4895</v>
+        <v>57.491300000000003</v>
       </c>
       <c r="F80">
-        <v>1.4E-3</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="G80">
-        <v>2.1600000000000001E-2</v>
+        <v>0.60399999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,13 +8385,13 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>76.246600000000001</v>
+        <v>76.213099999999997</v>
       </c>
       <c r="F81">
-        <v>0.19570000000000001</v>
+        <v>0.27250000000000002</v>
       </c>
       <c r="G81">
-        <v>0.1351</v>
+        <v>0.42309999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>87.387600000000006</v>
+        <v>87.301000000000002</v>
       </c>
       <c r="F82">
-        <v>0.29830000000000001</v>
+        <v>0.74709999999999999</v>
       </c>
       <c r="G82">
-        <v>9.9000000000000005E-2</v>
+        <v>0.13300000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>93.460700000000003</v>
+        <v>93.405000000000001</v>
       </c>
       <c r="F83">
-        <v>0.31559999999999999</v>
+        <v>4.7699999999999999E-2</v>
       </c>
       <c r="G83">
-        <v>1.0500000000000001E-2</v>
+        <v>6.6400000000000001E-2</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9366,13 +8454,13 @@
         <v>2</v>
       </c>
       <c r="E85">
-        <v>3.1701999999999999</v>
+        <v>3.1627000000000001</v>
       </c>
       <c r="F85">
-        <v>0.20419999999999999</v>
+        <v>0.26350000000000001</v>
       </c>
       <c r="G85">
-        <v>0.54459999999999997</v>
+        <v>0.28589999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,13 +8500,13 @@
         <v>8</v>
       </c>
       <c r="E87">
-        <v>60.939599999999999</v>
+        <v>60.939100000000003</v>
       </c>
       <c r="F87">
-        <v>1.1295999999999999</v>
+        <v>1.1296999999999999</v>
       </c>
       <c r="G87">
-        <v>0.1986</v>
+        <v>0.20019999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>78.239199999999997</v>
+        <v>78.240300000000005</v>
       </c>
       <c r="F88">
-        <v>0.49909999999999999</v>
+        <v>0.35720000000000002</v>
       </c>
       <c r="G88">
-        <v>0.1249</v>
+        <v>0.18509999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>88.455399999999997</v>
+        <v>88.115600000000001</v>
       </c>
       <c r="F89">
-        <v>0.39650000000000002</v>
+        <v>0.75890000000000002</v>
       </c>
       <c r="G89">
-        <v>0.1234</v>
+        <v>0.38750000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9481,13 +8569,13 @@
         <v>2</v>
       </c>
       <c r="E91">
-        <v>0.12189999999999999</v>
+        <v>0.1153</v>
       </c>
       <c r="F91">
-        <v>7.6399999999999996E-2</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="G91">
-        <v>0.185</v>
+        <v>0.2913</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -9504,13 +8592,13 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <v>23.5426</v>
+        <v>23.5322</v>
       </c>
       <c r="F92">
-        <v>0.67330000000000001</v>
+        <v>0.66290000000000004</v>
       </c>
       <c r="G92">
-        <v>3.3E-3</v>
+        <v>1.37E-2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8615,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>47.199800000000003</v>
+        <v>47.556199999999997</v>
       </c>
       <c r="F93">
-        <v>1.4937</v>
+        <v>1.8501000000000001</v>
       </c>
       <c r="G93">
-        <v>0.75990000000000002</v>
+        <v>0.32840000000000003</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>66.995500000000007</v>
+        <v>67.404499999999999</v>
       </c>
       <c r="F94">
-        <v>3.5150000000000001</v>
+        <v>1.2707999999999999</v>
       </c>
       <c r="G94">
-        <v>0.26450000000000001</v>
+        <v>0.56030000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>81.934100000000001</v>
+        <v>81.595600000000005</v>
       </c>
       <c r="F95">
-        <v>0.3921</v>
+        <v>1.4548000000000001</v>
       </c>
       <c r="G95">
-        <v>5.7299999999999997E-2</v>
+        <v>0.18990000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9602,7 +8690,7 @@
         <v>2.3800000000000002E-2</v>
       </c>
       <c r="G97">
-        <v>3.3999999999999998E-3</v>
+        <v>9.1700000000000004E-2</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -9619,13 +8707,13 @@
         <v>4</v>
       </c>
       <c r="E98">
-        <v>22.712900000000001</v>
+        <v>22.541599999999999</v>
       </c>
       <c r="F98">
-        <v>0.4904</v>
+        <v>0.31909999999999999</v>
       </c>
       <c r="G98">
-        <v>7.3000000000000001E-3</v>
+        <v>0.17860000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -9642,13 +8730,13 @@
         <v>8</v>
       </c>
       <c r="E99">
-        <v>46.150799999999997</v>
+        <v>46.567300000000003</v>
       </c>
       <c r="F99">
-        <v>1.2388999999999999</v>
+        <v>1.6564000000000001</v>
       </c>
       <c r="G99">
-        <v>0.74109999999999998</v>
+        <v>0.40260000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>66.7607</v>
+        <v>66.739699999999999</v>
       </c>
       <c r="F100">
-        <v>6.9599999999999995E-2</v>
+        <v>2.7446999999999999</v>
       </c>
       <c r="G100">
-        <v>0.34260000000000002</v>
+        <v>0.53700000000000003</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>81.151799999999994</v>
+        <v>80.933400000000006</v>
       </c>
       <c r="F101">
-        <v>1.0084</v>
+        <v>0.31990000000000002</v>
       </c>
       <c r="G101">
-        <v>0.35060000000000002</v>
+        <v>0.50419999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>